<commit_message>
added some features from past week
</commit_message>
<xml_diff>
--- a/партии стран.xlsx
+++ b/партии стран.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krizhownik\Documents\Paradox Interactive\Hearts of Iron IV\mod\bofanski_ik\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F145727-7837-4D43-855F-5C3487F90E36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413D7D89-B6B0-40BD-B398-E81901910B93}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAE94B5B-5941-470B-90AF-880B13026B7C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>страна</t>
   </si>
@@ -223,6 +223,27 @@
   </si>
   <si>
     <t>Святой Синод</t>
+  </si>
+  <si>
+    <t>Коммунистическая партия</t>
+  </si>
+  <si>
+    <t>Единый Пайноплус</t>
+  </si>
+  <si>
+    <t>Соц.-дем. Партия</t>
+  </si>
+  <si>
+    <t>Совет крестьянских общин</t>
+  </si>
+  <si>
+    <t>Союз эгоистов</t>
+  </si>
+  <si>
+    <t>Левая Интеелегенция</t>
+  </si>
+  <si>
+    <t>Партия Равенства</t>
   </si>
 </sst>
 </file>
@@ -650,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4724E4-08BC-4C40-8B94-7075D03B3E9E}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,6 +868,21 @@
       <c r="I7" t="s">
         <v>62</v>
       </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1010,6 +1046,9 @@
       <c r="B24" t="s">
         <v>53</v>
       </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
@@ -1033,6 +1072,9 @@
       </c>
       <c r="B27" t="s">
         <v>44</v>
+      </c>
+      <c r="G27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>